<commit_message>
first code parts of orbit calculation
</commit_message>
<xml_diff>
--- a/Work/432_finalPorject_task1.xlsx
+++ b/Work/432_finalPorject_task1.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simte\Documents\PHY432\final-2024-the-skywalkers\Work\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAE68AE-8CF9-4FA8-826A-F5906C75E905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Mass(kg)</t>
   </si>
@@ -68,31 +77,80 @@
   </si>
   <si>
     <t>https://starwars.fandom.com/wiki/DS-2_Death_Star_II_Mobile_Battle_Station</t>
+  </si>
+  <si>
+    <t>Final Project 432: Gravitational Impacts of the Death Star on Endor and Earth-like planets</t>
+  </si>
+  <si>
+    <t>Team: The Skywalkers</t>
+  </si>
+  <si>
+    <t>Collection of necessary parameters</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Nr. Estimation</t>
+  </si>
+  <si>
+    <t>https://www.tdgutierrez.com/2017/07/28/part-ii-mass-of-the-death-star-in-episode-iv/</t>
+  </si>
+  <si>
+    <t>Star Killer Base</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,54 +158,60 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -337,163 +401,217 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="18.13"/>
-    <col customWidth="1" min="5" max="5" width="15.63"/>
-    <col customWidth="1" min="8" max="8" width="45.88"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J7" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>7.52E23</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2450.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>402.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>3.0E7</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="C8" s="2">
+        <v>7.5200000000000003E+23</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2450</v>
+      </c>
+      <c r="E8" s="1">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1">
+        <v>402</v>
+      </c>
+      <c r="G8" s="2">
+        <v>30000000</v>
+      </c>
+      <c r="H8" s="1">
         <v>8.35</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L8" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
-        <v>5.97E24</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6357.0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>365.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>8.1E9</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="C9" s="2">
+        <v>5.9700000000000003E+24</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6357</v>
+      </c>
+      <c r="E9" s="1">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1">
+        <v>365</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8100000000</v>
+      </c>
+      <c r="H9" s="1">
         <v>9.81</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="7" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
-        <v>7.35E22</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1737.0</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C10" s="2">
+        <v>7.3500000000000001E+22</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1737</v>
+      </c>
+      <c r="E10" s="1">
         <v>655.7</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F10" s="1">
         <v>27.3</v>
       </c>
-      <c r="F4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
         <v>1.62</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>750000.0</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>80</v>
+      </c>
+      <c r="G11" s="1">
+        <v>750000</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J11" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2.8000000000000002E+23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I2"/>
-    <hyperlink r:id="rId2" location=":~:text=Plugging%20in%20our%20values%20gives,the%20mass%20of%20the%20Moon.&amp;text=This%20is%20a%20simple%20calculation,12%2C191%20kg/m%5E3." ref="J2"/>
-    <hyperlink r:id="rId3" ref="K2"/>
-    <hyperlink r:id="rId4" ref="I3"/>
-    <hyperlink r:id="rId5" ref="I4"/>
-    <hyperlink r:id="rId6" ref="I5"/>
+    <hyperlink ref="J8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K8" r:id="rId6" location=":~:text=Plugging%20in%20our%20values%20gives,the%20mass%20of%20the%20Moon.&amp;text=This%20is%20a%20simple%20calculation,12%2C191%20kg/m%5E3." xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
endor orbits finish, other slight corrections
</commit_message>
<xml_diff>
--- a/Work/432_finalPorject_task1.xlsx
+++ b/Work/432_finalPorject_task1.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simte\Documents\PHY432\final-2024-the-skywalkers\Work\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BFCA53-2750-4CD5-BC6E-8CA19B1A585B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -82,9 +91,6 @@
     <t>https://starwars.fandom.com/wiki/Endor_(planet)/Legends</t>
   </si>
   <si>
-    <t>Death Star 1</t>
-  </si>
-  <si>
     <t>6.2e32 J/s power output blast from their superlasers</t>
   </si>
   <si>
@@ -97,9 +103,6 @@
     <t>Death Star 1-2</t>
   </si>
   <si>
-    <t>Death Star 2</t>
-  </si>
-  <si>
     <t>Made up of Quadanium steel(made up steel(Steel density = 7,859 kg/m^2))</t>
   </si>
   <si>
@@ -122,31 +125,42 @@
   </si>
   <si>
     <t>https://www.scientificamerican.com/article/no-endor-in-sight-habitable-exomoons-may-be-rare/</t>
+  </si>
+  <si>
+    <t>Death Star B</t>
+  </si>
+  <si>
+    <t>Death Star A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,54 +168,46 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -391,26 +397,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.75"/>
-    <col customWidth="1" min="4" max="4" width="18.13"/>
-    <col customWidth="1" min="5" max="5" width="15.63"/>
-    <col customWidth="1" min="8" max="8" width="5.75"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,75 +447,75 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>7.52E23</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2450.0</v>
+        <v>7.5200000000000003E+23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2450</v>
       </c>
       <c r="D2" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1">
-        <v>402.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>3.0E7</v>
-      </c>
-      <c r="G2" s="5">
+        <v>402</v>
+      </c>
+      <c r="F2" s="2">
+        <v>30000000</v>
+      </c>
+      <c r="G2" s="1">
         <v>8.35</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <v>5.97E24</v>
+        <v>5.9700000000000003E+24</v>
       </c>
       <c r="C3" s="1">
-        <v>6357.0</v>
+        <v>6357</v>
       </c>
       <c r="D3" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1">
-        <v>365.0</v>
+        <v>365</v>
       </c>
       <c r="F3" s="2">
-        <v>8.1E9</v>
+        <v>8100000000</v>
       </c>
       <c r="G3" s="1">
         <v>9.81</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>7.35E22</v>
+        <v>7.3500000000000001E+22</v>
       </c>
       <c r="C4" s="1">
-        <v>1737.0</v>
+        <v>1737</v>
       </c>
       <c r="D4" s="1">
         <v>655.7</v>
@@ -513,164 +524,166 @@
         <v>27.3</v>
       </c>
       <c r="F4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>1.62</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>1.6E22</v>
+        <v>1.6E+22</v>
       </c>
       <c r="C5" s="1">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="F5" s="2"/>
       <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="2">
-        <v>1.37E24</v>
+        <v>1.3699999999999999E+24</v>
       </c>
       <c r="C6" s="1">
-        <v>415.0</v>
+        <v>415</v>
       </c>
       <c r="F6" s="2"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>2.01E27</v>
+        <v>2.01E+27</v>
       </c>
       <c r="C7" s="1">
-        <v>74000.0</v>
+        <v>74000</v>
       </c>
       <c r="F7" s="2"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2">
-        <v>2.8E23</v>
+        <v>2.8000000000000002E+23</v>
       </c>
       <c r="C8" s="1">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="J8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="7" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1E+18</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2471647</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2471647.0</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="B11" s="2">
+        <v>1.9889999999999999E+30</v>
+      </c>
+      <c r="C11" s="1">
+        <v>696000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1.989E30</v>
-      </c>
-      <c r="C11" s="1">
-        <v>696000.0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>275.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2">
-        <v>1.49E8</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>149000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -678,27 +691,27 @@
         <v>14</v>
       </c>
       <c r="C20" s="2">
-        <v>384000.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>384000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2">
+        <v>25000</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="2">
-        <v>25000.0</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -706,28 +719,28 @@
         <v>21</v>
       </c>
       <c r="C22" s="2">
-        <v>1.25E7</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>36</v>
+        <v>12500000</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I2"/>
-    <hyperlink r:id="rId2" location=":~:text=Plugging%20in%20our%20values%20gives,the%20mass%20of%20the%20Moon.&amp;text=This%20is%20a%20simple%20calculation,12%2C191%20kg/m%5E3." ref="J2"/>
-    <hyperlink r:id="rId3" ref="K2"/>
-    <hyperlink r:id="rId4" ref="I3"/>
-    <hyperlink r:id="rId5" ref="I4"/>
-    <hyperlink r:id="rId6" location=":~:text=With%20a%20diameter%20of%20660km,1.6%20%C3%97%201022%20kg." ref="I5"/>
-    <hyperlink r:id="rId7" ref="I6"/>
-    <hyperlink r:id="rId8" ref="I7"/>
-    <hyperlink r:id="rId9" ref="I8"/>
-    <hyperlink r:id="rId10" location=":~:text=We%20found%20that%20the%20Death,therefore%2C%20equal%20to%2060%20km." ref="J8"/>
-    <hyperlink r:id="rId11" ref="I10"/>
-    <hyperlink r:id="rId12" ref="I21"/>
-    <hyperlink r:id="rId13" ref="I22"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" location=":~:text=Plugging%20in%20our%20values%20gives,the%20mass%20of%20the%20Moon.&amp;text=This%20is%20a%20simple%20calculation,12%2C191%20kg/m%5E3." xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I5" r:id="rId6" location=":~:text=With%20a%20diameter%20of%20660km,1.6%20%C3%97%201022%20kg." xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J8" r:id="rId10" location=":~:text=We%20found%20that%20the%20Death,therefore%2C%20equal%20to%2060%20km." xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I21" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
   </hyperlinks>
-  <drawing r:id="rId14"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>